<commit_message>
hybrid inout EXP version
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-15.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-15.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inflow vs outflow" sheetId="1" r:id="rId1"/>
+    <sheet name="hybrid InOut" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -88,6 +89,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24 outflow.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 InOut.csv)</t>
   </si>
 </sst>
 </file>
@@ -444,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,4 +1775,463 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:E57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3" t="e">
+        <f>AVERAGE(D5:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E56" s="3" t="e">
+        <f>AVERAGE(E5:E54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3" t="e">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E57" s="3" t="e">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hybrid InOut test-15 without popsize
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-15.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-15.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 InOut.csv) without popsize</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:R57"/>
+  <dimension ref="C3:V57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,9 +1811,11 @@
     <col min="15" max="15" width="11.140625" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" customWidth="1"/>
     <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" customWidth="1"/>
+    <col min="22" max="22" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1827,8 +1832,12 @@
         <v>27</v>
       </c>
       <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -1860,8 +1869,15 @@
       <c r="R4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -1901,8 +1917,17 @@
       <c r="R5" s="3">
         <v>94.979852249832092</v>
       </c>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T5" s="2">
+        <v>1</v>
+      </c>
+      <c r="U5" s="3">
+        <v>42.931676042356067</v>
+      </c>
+      <c r="V5" s="3">
+        <v>113.2102380952381</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -1946,8 +1971,18 @@
       <c r="R6" s="3">
         <v>96.483243787777027</v>
       </c>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T6" s="2">
+        <f>T5+1</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="3">
+        <v>42.401762078094002</v>
+      </c>
+      <c r="V6" s="3">
+        <v>115.546798941799</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -1991,8 +2026,18 @@
       <c r="R7" s="3">
         <v>97.748844862323708</v>
       </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T7" s="2">
+        <f t="shared" ref="T7:T54" si="4">T6+1</f>
+        <v>3</v>
+      </c>
+      <c r="U7" s="3">
+        <v>42.936035737921912</v>
+      </c>
+      <c r="V7" s="3">
+        <v>110.5523743386243</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2036,8 +2081,18 @@
       <c r="R8" s="3">
         <v>97.348623237071862</v>
       </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T8" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="U8" s="3">
+        <v>42.771255790867002</v>
+      </c>
+      <c r="V8" s="3">
+        <v>107.8129828042328</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2081,8 +2136,18 @@
       <c r="R9" s="3">
         <v>99.289751511081249</v>
       </c>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T9" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="U9" s="3">
+        <v>42.649005625413658</v>
+      </c>
+      <c r="V9" s="3">
+        <v>115.3442195767196</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2126,8 +2191,18 @@
       <c r="R10" s="3">
         <v>93.387716588314291</v>
       </c>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T10" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="U10" s="3">
+        <v>42.60552614162809</v>
+      </c>
+      <c r="V10" s="3">
+        <v>116.4408333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2171,8 +2246,18 @@
       <c r="R11" s="3">
         <v>100.25349227669579</v>
       </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T11" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="U11" s="3">
+        <v>42.811275645268047</v>
+      </c>
+      <c r="V11" s="3">
+        <v>110.5954034391534</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2216,8 +2301,18 @@
       <c r="R12" s="3">
         <v>98.036111484217571</v>
       </c>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T12" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="U12" s="3">
+        <v>41.903606882859059</v>
+      </c>
+      <c r="V12" s="3">
+        <v>114.02434523809519</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2261,8 +2356,18 @@
       <c r="R13" s="3">
         <v>98.474016118200126</v>
       </c>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T13" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="U13" s="3">
+        <v>42.014829583057598</v>
+      </c>
+      <c r="V13" s="3">
+        <v>114.1235978835979</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2306,8 +2411,18 @@
       <c r="R14" s="3">
         <v>100.2977165883143</v>
       </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T14" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="U14" s="3">
+        <v>42.643059232296523</v>
+      </c>
+      <c r="V14" s="3">
+        <v>113.8430158730159</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2351,8 +2466,18 @@
       <c r="R15" s="3">
         <v>102.08296171927471</v>
       </c>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T15" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="U15" s="3">
+        <v>42.990335870284589</v>
+      </c>
+      <c r="V15" s="3">
+        <v>113.8879960317461</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2396,8 +2521,18 @@
       <c r="R16" s="3">
         <v>96.635708529214241</v>
       </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T16" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="U16" s="3">
+        <v>42.158866644606228</v>
+      </c>
+      <c r="V16" s="3">
+        <v>110.2759920634921</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2441,8 +2576,18 @@
       <c r="R17" s="3">
         <v>94.58910006715918</v>
       </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T17" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="U17" s="3">
+        <v>42.628631700860382</v>
+      </c>
+      <c r="V17" s="3">
+        <v>113.8253108465608</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2486,8 +2631,18 @@
       <c r="R18" s="3">
         <v>97.300141034251169</v>
       </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T18" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="U18" s="3">
+        <v>43.418524156187978</v>
+      </c>
+      <c r="V18" s="3">
+        <v>107.7265277777778</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2531,8 +2686,18 @@
       <c r="R19" s="3">
         <v>94.231511081262582</v>
       </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T19" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="U19" s="3">
+        <v>43.359371277299807</v>
+      </c>
+      <c r="V19" s="3">
+        <v>106.89069444444451</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2576,8 +2741,18 @@
       <c r="R20" s="3">
         <v>103.1834654130289</v>
       </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T20" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="U20" s="3">
+        <v>42.737356055592343</v>
+      </c>
+      <c r="V20" s="3">
+        <v>114.1889682539683</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2621,8 +2796,18 @@
       <c r="R21" s="3">
         <v>93.387662860980527</v>
       </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T21" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="U21" s="3">
+        <v>42.960213434811408</v>
+      </c>
+      <c r="V21" s="3">
+        <v>115.0267724867725</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2666,8 +2851,18 @@
       <c r="R22" s="3">
         <v>96.045970449966404</v>
       </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T22" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="U22" s="3">
+        <v>43.040565850430198</v>
+      </c>
+      <c r="V22" s="3">
+        <v>105.3709060846561</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2711,8 +2906,18 @@
       <c r="R23" s="3">
         <v>99.390738750839489</v>
       </c>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T23" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="U23" s="3">
+        <v>42.544645929847803</v>
+      </c>
+      <c r="V23" s="3">
+        <v>115.0999338624339</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2756,8 +2961,18 @@
       <c r="R24" s="3">
         <v>96.450214909335131</v>
       </c>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T24" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="U24" s="3">
+        <v>42.708072468563913</v>
+      </c>
+      <c r="V24" s="3">
+        <v>111.1607473544974</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2801,8 +3016,18 @@
       <c r="R25" s="3">
         <v>98.2770920080591</v>
       </c>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T25" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="U25" s="3">
+        <v>44.195410324288559</v>
+      </c>
+      <c r="V25" s="3">
+        <v>102.92511243386249</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2846,8 +3071,18 @@
       <c r="R26" s="3">
         <v>97.128663532572176</v>
       </c>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T26" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="U26" s="3">
+        <v>42.539669093315688</v>
+      </c>
+      <c r="V26" s="3">
+        <v>119.1875330687831</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2891,8 +3126,18 @@
       <c r="R27" s="3">
         <v>96.354936198791123</v>
       </c>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T27" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="U27" s="3">
+        <v>43.169199205823958</v>
+      </c>
+      <c r="V27" s="3">
+        <v>113.3158399470899</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2936,8 +3181,18 @@
       <c r="R28" s="3">
         <v>98.824002686366683</v>
       </c>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T28" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="U28" s="3">
+        <v>43.113949371277307</v>
+      </c>
+      <c r="V28" s="3">
+        <v>110.1356415343916</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2981,8 +3236,18 @@
       <c r="R29" s="3">
         <v>99.533089321692415</v>
       </c>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T29" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="U29" s="3">
+        <v>43.018021178027787</v>
+      </c>
+      <c r="V29" s="3">
+        <v>114.11869047619049</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3026,8 +3291,18 @@
       <c r="R30" s="3">
         <v>95.2527333781061</v>
       </c>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T30" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="U30" s="3">
+        <v>42.736968894771699</v>
+      </c>
+      <c r="V30" s="3">
+        <v>113.6920502645503</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3071,8 +3346,18 @@
       <c r="R31" s="3">
         <v>94.601356615177977</v>
       </c>
-    </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T31" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="U31" s="3">
+        <v>42.74030939774984</v>
+      </c>
+      <c r="V31" s="3">
+        <v>109.94958333333339</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3116,8 +3401,18 @@
       <c r="R32" s="3">
         <v>100.1417058428475</v>
       </c>
-    </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T32" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="U32" s="3">
+        <v>42.273403375248201</v>
+      </c>
+      <c r="V32" s="3">
+        <v>113.30990740740739</v>
+      </c>
+    </row>
+    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3161,8 +3456,18 @@
       <c r="R33" s="3">
         <v>94.03676292813968</v>
       </c>
-    </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T33" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="U33" s="3">
+        <v>42.639659166115173</v>
+      </c>
+      <c r="V33" s="3">
+        <v>108.0595502645503</v>
+      </c>
+    </row>
+    <row r="34" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3206,8 +3511,18 @@
       <c r="R34" s="3">
         <v>97.004472800537258</v>
       </c>
-    </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T34" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="U34" s="3">
+        <v>43.352210456651243</v>
+      </c>
+      <c r="V34" s="3">
+        <v>108.39755952380951</v>
+      </c>
+    </row>
+    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3251,8 +3566,18 @@
       <c r="R35" s="3">
         <v>93.270080591000664</v>
       </c>
-    </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T35" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="U35" s="3">
+        <v>42.383409993381903</v>
+      </c>
+      <c r="V35" s="3">
+        <v>107.8047883597884</v>
+      </c>
+    </row>
+    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3296,8 +3621,18 @@
       <c r="R36" s="3">
         <v>97.239603760913383</v>
       </c>
-    </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T36" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="U36" s="3">
+        <v>42.466308735936487</v>
+      </c>
+      <c r="V36" s="3">
+        <v>109.04320105820111</v>
+      </c>
+    </row>
+    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3341,8 +3676,18 @@
       <c r="R37" s="3">
         <v>99.326984553391526</v>
       </c>
-    </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T37" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="U37" s="3">
+        <v>42.137531436135021</v>
+      </c>
+      <c r="V37" s="3">
+        <v>107.7612830687831</v>
+      </c>
+    </row>
+    <row r="38" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3386,8 +3731,18 @@
       <c r="R38" s="3">
         <v>103.0932505036937</v>
       </c>
-    </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T38" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="U38" s="3">
+        <v>43.304746856386508</v>
+      </c>
+      <c r="V38" s="3">
+        <v>103.34669312169321</v>
+      </c>
+    </row>
+    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3431,8 +3786,18 @@
       <c r="R39" s="3">
         <v>101.5870718603089</v>
       </c>
-    </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T39" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="U39" s="3">
+        <v>42.990734612839198</v>
+      </c>
+      <c r="V39" s="3">
+        <v>111.28826058201059</v>
+      </c>
+    </row>
+    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3476,8 +3841,18 @@
       <c r="R40" s="3">
         <v>97.55313633310945</v>
       </c>
-    </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T40" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="U40" s="3">
+        <v>42.988168431502309</v>
+      </c>
+      <c r="V40" s="3">
+        <v>111.2536375661376</v>
+      </c>
+    </row>
+    <row r="41" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3521,8 +3896,18 @@
       <c r="R41" s="3">
         <v>96.219798522498323</v>
       </c>
-    </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T41" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="U41" s="3">
+        <v>42.930206816677703</v>
+      </c>
+      <c r="V41" s="3">
+        <v>109.44046957671959</v>
+      </c>
+    </row>
+    <row r="42" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3566,8 +3951,18 @@
       <c r="R42" s="3">
         <v>97.743116185359298</v>
       </c>
-    </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T42" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="U42" s="3">
+        <v>43.137845797485113</v>
+      </c>
+      <c r="V42" s="3">
+        <v>105.8178108465609</v>
+      </c>
+    </row>
+    <row r="43" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3611,8 +4006,18 @@
       <c r="R43" s="3">
         <v>97.416400268636664</v>
       </c>
-    </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T43" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="U43" s="3">
+        <v>42.529118133686303</v>
+      </c>
+      <c r="V43" s="3">
+        <v>113.2455291005291</v>
+      </c>
+    </row>
+    <row r="44" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3656,8 +4061,18 @@
       <c r="R44" s="3">
         <v>98.837897918065821</v>
       </c>
-    </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T44" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="U44" s="3">
+        <v>43.157554599602932</v>
+      </c>
+      <c r="V44" s="3">
+        <v>107.7580291005291</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3701,8 +4116,18 @@
       <c r="R45" s="3">
         <v>100.5845466756212</v>
       </c>
-    </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T45" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="U45" s="3">
+        <v>43.399030443414993</v>
+      </c>
+      <c r="V45" s="3">
+        <v>111.7703968253968</v>
+      </c>
+    </row>
+    <row r="46" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3746,8 +4171,18 @@
       <c r="R46" s="3">
         <v>101.0010611148422</v>
       </c>
-    </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T46" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="U46" s="3">
+        <v>42.909612839179367</v>
+      </c>
+      <c r="V46" s="3">
+        <v>110.6335714285714</v>
+      </c>
+    </row>
+    <row r="47" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3791,8 +4226,18 @@
       <c r="R47" s="3">
         <v>96.363955674949636</v>
       </c>
-    </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T47" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="U47" s="3">
+        <v>43.144440767703522</v>
+      </c>
+      <c r="V47" s="3">
+        <v>105.8499404761905</v>
+      </c>
+    </row>
+    <row r="48" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3836,8 +4281,18 @@
       <c r="R48" s="3">
         <v>96.194110141034244</v>
       </c>
-    </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T48" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="U48" s="3">
+        <v>42.800592322964953</v>
+      </c>
+      <c r="V48" s="3">
+        <v>110.7671494708995</v>
+      </c>
+    </row>
+    <row r="49" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3881,8 +4336,18 @@
       <c r="R49" s="3">
         <v>96.968206850235063</v>
       </c>
-    </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T49" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="U49" s="3">
+        <v>41.952918596955683</v>
+      </c>
+      <c r="V49" s="3">
+        <v>113.86871693121689</v>
+      </c>
+    </row>
+    <row r="50" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3926,8 +4391,18 @@
       <c r="R50" s="3">
         <v>95.112108797850908</v>
       </c>
-    </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T50" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="U50" s="3">
+        <v>43.038198213103897</v>
+      </c>
+      <c r="V50" s="3">
+        <v>109.0930357142857</v>
+      </c>
+    </row>
+    <row r="51" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3971,8 +4446,18 @@
       <c r="R51" s="3">
         <v>93.650114170584288</v>
       </c>
-    </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T51" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="U51" s="3">
+        <v>43.012478491065522</v>
+      </c>
+      <c r="V51" s="3">
+        <v>110.2868187830688</v>
+      </c>
+    </row>
+    <row r="52" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4016,8 +4501,18 @@
       <c r="R52" s="3">
         <v>100.5610275352585</v>
       </c>
-    </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T52" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="U52" s="3">
+        <v>42.814978491065517</v>
+      </c>
+      <c r="V52" s="3">
+        <v>106.0479563492064</v>
+      </c>
+    </row>
+    <row r="53" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4061,8 +4556,18 @@
       <c r="R53" s="3">
         <v>96.358596373404978</v>
       </c>
-    </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T53" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="U53" s="3">
+        <v>43.11228821972206</v>
+      </c>
+      <c r="V53" s="3">
+        <v>107.2581084656085</v>
+      </c>
+    </row>
+    <row r="54" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4106,8 +4611,18 @@
       <c r="R54" s="3">
         <v>100.1011820013432</v>
       </c>
-    </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T54" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="U54" s="3">
+        <v>42.816221045665131</v>
+      </c>
+      <c r="V54" s="3">
+        <v>112.7418849206349</v>
+      </c>
+    </row>
+    <row r="56" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -4156,8 +4671,19 @@
         <f>AVERAGE(R5:R54)</f>
         <v>97.598678173270599</v>
       </c>
-    </row>
-    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="T56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U56" s="3">
+        <f>AVERAGE(U5:U54)</f>
+        <v>42.82039602911982</v>
+      </c>
+      <c r="V56" s="3">
+        <f>AVERAGE(V5:V54)</f>
+        <v>110.86232817460321</v>
+      </c>
+    </row>
+    <row r="57" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -4205,6 +4731,17 @@
       <c r="R57" s="3">
         <f>_xlfn.STDEV.S(R5:R54)</f>
         <v>2.5439019153472042</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U57" s="3">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
+        <v>0.42174306573187897</v>
+      </c>
+      <c r="V57" s="3">
+        <f>_xlfn.STDEV.S(V5:V54)</f>
+        <v>3.5469345251178352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-16 for total saldo
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-15.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-15.xlsx
@@ -1807,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:V57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -4818,7 +4818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="X46" sqref="X46"/>
     </sheetView>
   </sheetViews>

</xml_diff>